<commit_message>
track  + train + train controlelr integrated
</commit_message>
<xml_diff>
--- a/TrackModel/trackData/GreenLine.xlsx
+++ b/TrackModel/trackData/GreenLine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/njm130_pitt_edu/Documents/Documents/1140 Trains/trains/TrackModel/trackData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b71eb1e12f3a2cab/Documents/2024-2025/ECE 1140/Git Hub/trains/TrackModel/trackData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{F5A40FCF-132B-4770-BC5C-2DBF2C123779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F4B216E-F8B0-4AA0-955C-BC48A94DAF40}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{F5A40FCF-132B-4770-BC5C-2DBF2C123779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D542BE91-CC21-4B40-B0C6-F29012B62AF1}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="107">
   <si>
     <t>Line</t>
   </si>
@@ -239,13 +239,124 @@
     <t>Non</t>
   </si>
   <si>
-    <t>beep</t>
+    <t>Yard</t>
   </si>
   <si>
-    <t>boop</t>
+    <t>B1,2,Pioneer</t>
   </si>
   <si>
-    <t>Yard</t>
+    <t>B2,2,Pioneer</t>
+  </si>
+  <si>
+    <t>B3,2,Edgebrook</t>
+  </si>
+  <si>
+    <t>B4,2,Edgebrook</t>
+  </si>
+  <si>
+    <t>B5,3,Lebron</t>
+  </si>
+  <si>
+    <t>B6,3,Lebron</t>
+  </si>
+  <si>
+    <t>B7,3,Whited</t>
+  </si>
+  <si>
+    <t>B8,3,Whited</t>
+  </si>
+  <si>
+    <t>B9,2,South Bank</t>
+  </si>
+  <si>
+    <t>B10,2,South Bank</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>B11,1,Central</t>
+  </si>
+  <si>
+    <t>B12,1,Central</t>
+  </si>
+  <si>
+    <t>B13,1,Inglewood</t>
+  </si>
+  <si>
+    <t>B14,1,Inglewood</t>
+  </si>
+  <si>
+    <t>B15,1,Overbrook</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>B16,1,Overbrook</t>
+  </si>
+  <si>
+    <t>B17,1,Glenbury</t>
+  </si>
+  <si>
+    <t>B18,1,Glenbury</t>
+  </si>
+  <si>
+    <t>B19,1,Dormont</t>
+  </si>
+  <si>
+    <t>B20,1,Dormont</t>
+  </si>
+  <si>
+    <t>B21,3,Mt Lebanon</t>
+  </si>
+  <si>
+    <t>B22,3,Mt Lebanon</t>
+  </si>
+  <si>
+    <t>B23,2,Mt Poplar</t>
+  </si>
+  <si>
+    <t>B24,2,Mt Poplar</t>
+  </si>
+  <si>
+    <t>B25,2,Castle Shannon</t>
+  </si>
+  <si>
+    <t>B26,2,Castle Shannon</t>
+  </si>
+  <si>
+    <t>B27,1,Dormont</t>
+  </si>
+  <si>
+    <t>B28,1,Dormont</t>
+  </si>
+  <si>
+    <t>B29,1,Glenbury</t>
+  </si>
+  <si>
+    <t>B30,1,Glenbury</t>
+  </si>
+  <si>
+    <t>B31,1,Overbrook</t>
+  </si>
+  <si>
+    <t>B32,1,Overbrook</t>
+  </si>
+  <si>
+    <t>B33,2,Inglewood</t>
+  </si>
+  <si>
+    <t>B34,2,Inglewood</t>
+  </si>
+  <si>
+    <t>B35,1,Central</t>
+  </si>
+  <si>
+    <t>B36,1,Central</t>
+  </si>
+  <si>
+    <t>T3</t>
   </si>
 </sst>
 </file>
@@ -672,9 +783,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8FE392-6FC0-4F53-90EE-920DCF161686}">
   <dimension ref="A1:T152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="102" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="P1" sqref="P1:P152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,7 +865,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="10">
         <v>0</v>
@@ -859,8 +970,8 @@
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="P3">
-        <v>0</v>
+      <c r="P3" t="s">
+        <v>68</v>
       </c>
       <c r="Q3" s="3">
         <v>0</v>
@@ -989,8 +1100,8 @@
       <c r="O5">
         <v>4</v>
       </c>
-      <c r="P5">
-        <v>0</v>
+      <c r="P5" t="s">
+        <v>69</v>
       </c>
       <c r="Q5" s="3">
         <v>0</v>
@@ -1314,8 +1425,8 @@
       <c r="O10">
         <v>9</v>
       </c>
-      <c r="P10">
-        <v>0</v>
+      <c r="P10" t="s">
+        <v>70</v>
       </c>
       <c r="Q10" s="3">
         <v>0</v>
@@ -1444,8 +1555,8 @@
       <c r="O12">
         <v>11</v>
       </c>
-      <c r="P12">
-        <v>0</v>
+      <c r="P12" t="s">
+        <v>71</v>
       </c>
       <c r="Q12" s="3">
         <v>0</v>
@@ -1769,8 +1880,8 @@
       <c r="O17">
         <v>16</v>
       </c>
-      <c r="P17">
-        <v>0</v>
+      <c r="P17" t="s">
+        <v>72</v>
       </c>
       <c r="Q17" s="3">
         <v>0</v>
@@ -1899,8 +2010,8 @@
       <c r="O19">
         <v>18</v>
       </c>
-      <c r="P19">
-        <v>0</v>
+      <c r="P19" t="s">
+        <v>73</v>
       </c>
       <c r="Q19" s="3">
         <v>0</v>
@@ -2159,8 +2270,8 @@
       <c r="O23">
         <v>22</v>
       </c>
-      <c r="P23">
-        <v>0</v>
+      <c r="P23" t="s">
+        <v>74</v>
       </c>
       <c r="Q23" s="3">
         <v>0</v>
@@ -2289,8 +2400,8 @@
       <c r="O25">
         <v>24</v>
       </c>
-      <c r="P25">
-        <v>0</v>
+      <c r="P25" t="s">
+        <v>75</v>
       </c>
       <c r="Q25" s="3">
         <v>0</v>
@@ -2744,8 +2855,8 @@
       <c r="O32">
         <v>31</v>
       </c>
-      <c r="P32">
-        <v>0</v>
+      <c r="P32" t="s">
+        <v>76</v>
       </c>
       <c r="Q32" s="3">
         <v>0</v>
@@ -2874,8 +2985,8 @@
       <c r="O34">
         <v>33</v>
       </c>
-      <c r="P34">
-        <v>0</v>
+      <c r="P34" t="s">
+        <v>77</v>
       </c>
       <c r="Q34" s="3">
         <v>0</v>
@@ -3134,8 +3245,8 @@
       <c r="O38">
         <v>37</v>
       </c>
-      <c r="P38">
-        <v>0</v>
+      <c r="P38" t="s">
+        <v>78</v>
       </c>
       <c r="Q38" s="3">
         <v>0</v>
@@ -3264,8 +3375,8 @@
       <c r="O40">
         <v>39</v>
       </c>
-      <c r="P40">
-        <v>0</v>
+      <c r="P40" t="s">
+        <v>79</v>
       </c>
       <c r="Q40" s="3">
         <v>0</v>
@@ -3394,8 +3505,8 @@
       <c r="O42">
         <v>41</v>
       </c>
-      <c r="P42">
-        <v>0</v>
+      <c r="P42" t="s">
+        <v>80</v>
       </c>
       <c r="Q42" s="3">
         <v>0</v>
@@ -3849,8 +3960,8 @@
       <c r="O49">
         <v>48</v>
       </c>
-      <c r="P49">
-        <v>0</v>
+      <c r="P49" t="s">
+        <v>81</v>
       </c>
       <c r="Q49" s="3">
         <v>0</v>
@@ -3979,8 +4090,8 @@
       <c r="O51">
         <v>50</v>
       </c>
-      <c r="P51">
-        <v>0</v>
+      <c r="P51" t="s">
+        <v>82</v>
       </c>
       <c r="Q51" s="3">
         <v>0</v>
@@ -4434,8 +4545,8 @@
       <c r="O58">
         <v>57</v>
       </c>
-      <c r="P58">
-        <v>0</v>
+      <c r="P58" t="s">
+        <v>83</v>
       </c>
       <c r="Q58" s="3">
         <v>0</v>
@@ -4499,8 +4610,8 @@
       <c r="O59" t="s">
         <v>57</v>
       </c>
-      <c r="P59">
-        <v>0</v>
+      <c r="P59" t="s">
+        <v>84</v>
       </c>
       <c r="Q59" s="3" t="b">
         <v>0</v>
@@ -4564,8 +4675,8 @@
       <c r="O60">
         <v>59</v>
       </c>
-      <c r="P60">
-        <v>0</v>
+      <c r="P60" t="s">
+        <v>85</v>
       </c>
       <c r="Q60" s="3">
         <v>0</v>
@@ -4954,8 +5065,8 @@
       <c r="O66">
         <v>65</v>
       </c>
-      <c r="P66">
-        <v>0</v>
+      <c r="P66" t="s">
+        <v>86</v>
       </c>
       <c r="Q66" s="3">
         <v>0</v>
@@ -5084,8 +5195,8 @@
       <c r="O68">
         <v>67</v>
       </c>
-      <c r="P68">
-        <v>0</v>
+      <c r="P68" t="s">
+        <v>87</v>
       </c>
       <c r="Q68" s="3">
         <v>0</v>
@@ -5474,8 +5585,8 @@
       <c r="O74">
         <v>73</v>
       </c>
-      <c r="P74">
-        <v>0</v>
+      <c r="P74" t="s">
+        <v>88</v>
       </c>
       <c r="Q74" s="3">
         <v>0</v>
@@ -5604,8 +5715,8 @@
       <c r="O76">
         <v>75</v>
       </c>
-      <c r="P76">
-        <v>0</v>
+      <c r="P76" t="s">
+        <v>89</v>
       </c>
       <c r="Q76" s="3">
         <v>0</v>
@@ -5734,8 +5845,8 @@
       <c r="O78">
         <v>77</v>
       </c>
-      <c r="P78">
-        <v>0</v>
+      <c r="P78" t="s">
+        <v>90</v>
       </c>
       <c r="Q78" s="3">
         <v>0</v>
@@ -5864,8 +5975,8 @@
       <c r="O80">
         <v>79</v>
       </c>
-      <c r="P80">
-        <v>0</v>
+      <c r="P80" t="s">
+        <v>91</v>
       </c>
       <c r="Q80" s="3">
         <v>0</v>
@@ -6450,7 +6561,7 @@
         <v>88</v>
       </c>
       <c r="P89" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="Q89" s="3">
         <v>0</v>
@@ -6577,7 +6688,7 @@
         <v>90</v>
       </c>
       <c r="P91" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="Q91" s="3">
         <v>0</v>
@@ -6966,8 +7077,8 @@
       <c r="O97">
         <v>96</v>
       </c>
-      <c r="P97">
-        <v>0</v>
+      <c r="P97" t="s">
+        <v>94</v>
       </c>
       <c r="Q97" s="3">
         <v>0</v>
@@ -7096,8 +7207,8 @@
       <c r="O99">
         <v>98</v>
       </c>
-      <c r="P99">
-        <v>0</v>
+      <c r="P99" t="s">
+        <v>95</v>
       </c>
       <c r="Q99" s="3">
         <v>0</v>
@@ -7551,8 +7662,8 @@
       <c r="O106">
         <v>105</v>
       </c>
-      <c r="P106">
-        <v>0</v>
+      <c r="P106" t="s">
+        <v>96</v>
       </c>
       <c r="Q106" s="3">
         <v>0</v>
@@ -7681,8 +7792,8 @@
       <c r="O108">
         <v>107</v>
       </c>
-      <c r="P108">
-        <v>0</v>
+      <c r="P108" t="s">
+        <v>97</v>
       </c>
       <c r="Q108" s="3">
         <v>0</v>
@@ -8136,8 +8247,8 @@
       <c r="O115">
         <v>114</v>
       </c>
-      <c r="P115">
-        <v>0</v>
+      <c r="P115" t="s">
+        <v>98</v>
       </c>
       <c r="Q115" s="3">
         <v>0</v>
@@ -8267,8 +8378,8 @@
       <c r="O117">
         <v>116</v>
       </c>
-      <c r="P117">
-        <v>0</v>
+      <c r="P117" t="s">
+        <v>99</v>
       </c>
       <c r="Q117" s="3">
         <v>0</v>
@@ -8722,8 +8833,8 @@
       <c r="O124">
         <v>123</v>
       </c>
-      <c r="P124">
-        <v>0</v>
+      <c r="P124" t="s">
+        <v>100</v>
       </c>
       <c r="Q124" s="3">
         <v>0</v>
@@ -8852,8 +8963,8 @@
       <c r="O126">
         <v>125</v>
       </c>
-      <c r="P126">
-        <v>0</v>
+      <c r="P126" t="s">
+        <v>101</v>
       </c>
       <c r="Q126" s="3">
         <v>0</v>
@@ -9307,8 +9418,8 @@
       <c r="O133">
         <v>132</v>
       </c>
-      <c r="P133">
-        <v>0</v>
+      <c r="P133" t="s">
+        <v>102</v>
       </c>
       <c r="Q133" s="3">
         <v>0</v>
@@ -9437,8 +9548,8 @@
       <c r="O135">
         <v>134</v>
       </c>
-      <c r="P135">
-        <v>0</v>
+      <c r="P135" t="s">
+        <v>103</v>
       </c>
       <c r="Q135" s="3">
         <v>0</v>
@@ -9892,8 +10003,8 @@
       <c r="O142">
         <v>141</v>
       </c>
-      <c r="P142">
-        <v>0</v>
+      <c r="P142" t="s">
+        <v>104</v>
       </c>
       <c r="Q142" s="3">
         <v>0</v>
@@ -10022,8 +10133,8 @@
       <c r="O144">
         <v>143</v>
       </c>
-      <c r="P144">
-        <v>0</v>
+      <c r="P144" t="s">
+        <v>105</v>
       </c>
       <c r="Q144" s="3">
         <v>0</v>
@@ -10087,8 +10198,8 @@
       <c r="O145">
         <v>144</v>
       </c>
-      <c r="P145">
-        <v>0</v>
+      <c r="P145" t="s">
+        <v>106</v>
       </c>
       <c r="Q145" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
adding timing and nate ecel change
</commit_message>
<xml_diff>
--- a/TrackModel/trackData/GreenLine.xlsx
+++ b/TrackModel/trackData/GreenLine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b71eb1e12f3a2cab/Documents/2024-2025/ECE 1140/Git Hub/trains/TrackModel/trackData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{F5A40FCF-132B-4770-BC5C-2DBF2C123779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D542BE91-CC21-4B40-B0C6-F29012B62AF1}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{F5A40FCF-132B-4770-BC5C-2DBF2C123779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F27E5A1D-2AD5-4579-825E-6061D9761D7E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
   </bookViews>
@@ -785,7 +785,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1:P152"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,10 +901,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="O2">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="P2">
         <v>0</v>

</xml_diff>

<commit_message>
working on getting one train to pioneer
</commit_message>
<xml_diff>
--- a/TrackModel/trackData/GreenLine.xlsx
+++ b/TrackModel/trackData/GreenLine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/njm130_pitt_edu/Documents/Documents/1140 Trains/trains/TrackModel/trackData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\TrackModel\trackData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="8_{F5A40FCF-132B-4770-BC5C-2DBF2C123779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AC96E52-64DD-4D76-B87A-96A2AAB63E1C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247374CB-8036-4A5A-8CE7-7EEC22481196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10284" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -203,9 +203,6 @@
     <t>Beacon Info</t>
   </si>
   <si>
-    <t>1, 12</t>
-  </si>
-  <si>
     <t>58, 0</t>
   </si>
   <si>
@@ -357,6 +354,9 @@
   </si>
   <si>
     <t>T3</t>
+  </si>
+  <si>
+    <t>12, 1</t>
   </si>
 </sst>
 </file>
@@ -784,8 +784,8 @@
   <dimension ref="A1:T152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="102" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A143" sqref="A143:XFD143"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,16 +849,16 @@
         <v>54</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="S1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -866,7 +866,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="10">
         <v>0</v>
@@ -966,13 +966,13 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q3" s="3">
         <v>0</v>
@@ -1102,7 +1102,7 @@
         <v>4</v>
       </c>
       <c r="P5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q5" s="3">
         <v>0</v>
@@ -1427,7 +1427,7 @@
         <v>9</v>
       </c>
       <c r="P10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q10" s="3">
         <v>0</v>
@@ -1557,7 +1557,7 @@
         <v>11</v>
       </c>
       <c r="P12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q12" s="3">
         <v>0</v>
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="O15">
         <v>14</v>
@@ -1882,7 +1882,7 @@
         <v>16</v>
       </c>
       <c r="P17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q17" s="3">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>0.5</v>
       </c>
       <c r="I18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2012,7 +2012,7 @@
         <v>18</v>
       </c>
       <c r="P19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q19" s="3">
         <v>0</v>
@@ -2272,7 +2272,7 @@
         <v>22</v>
       </c>
       <c r="P23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q23" s="3">
         <v>0</v>
@@ -2402,7 +2402,7 @@
         <v>24</v>
       </c>
       <c r="P25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q25" s="3">
         <v>0</v>
@@ -2724,7 +2724,7 @@
         <v>27</v>
       </c>
       <c r="O30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P30">
         <v>0</v>
@@ -2857,7 +2857,7 @@
         <v>31</v>
       </c>
       <c r="P32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q32" s="3">
         <v>0</v>
@@ -2987,7 +2987,7 @@
         <v>33</v>
       </c>
       <c r="P34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q34" s="3">
         <v>0</v>
@@ -3247,7 +3247,7 @@
         <v>37</v>
       </c>
       <c r="P38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q38" s="3">
         <v>0</v>
@@ -3377,7 +3377,7 @@
         <v>39</v>
       </c>
       <c r="P40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q40" s="3">
         <v>0</v>
@@ -3507,7 +3507,7 @@
         <v>41</v>
       </c>
       <c r="P42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q42" s="3">
         <v>0</v>
@@ -3962,7 +3962,7 @@
         <v>48</v>
       </c>
       <c r="P49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q49" s="3">
         <v>0</v>
@@ -4092,7 +4092,7 @@
         <v>50</v>
       </c>
       <c r="P51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q51" s="3">
         <v>0</v>
@@ -4547,7 +4547,7 @@
         <v>57</v>
       </c>
       <c r="P58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q58" s="3">
         <v>0</v>
@@ -4609,10 +4609,10 @@
         <v>56</v>
       </c>
       <c r="O59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q59" s="3" t="b">
         <v>0</v>
@@ -4677,7 +4677,7 @@
         <v>59</v>
       </c>
       <c r="P60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q60" s="3">
         <v>0</v>
@@ -4996,7 +4996,7 @@
         <v>0</v>
       </c>
       <c r="N65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O65">
         <v>64</v>
@@ -5067,7 +5067,7 @@
         <v>65</v>
       </c>
       <c r="P66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q66" s="3">
         <v>0</v>
@@ -5197,7 +5197,7 @@
         <v>67</v>
       </c>
       <c r="P68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q68" s="3">
         <v>0</v>
@@ -5587,7 +5587,7 @@
         <v>73</v>
       </c>
       <c r="P74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q74" s="3">
         <v>0</v>
@@ -5717,7 +5717,7 @@
         <v>75</v>
       </c>
       <c r="P76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q76" s="3">
         <v>0</v>
@@ -5847,7 +5847,7 @@
         <v>77</v>
       </c>
       <c r="P78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q78" s="3">
         <v>0</v>
@@ -5906,7 +5906,7 @@
         <v>0</v>
       </c>
       <c r="N79" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O79">
         <v>78</v>
@@ -5977,7 +5977,7 @@
         <v>79</v>
       </c>
       <c r="P80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q80" s="3">
         <v>0</v>
@@ -6429,7 +6429,7 @@
         <v>84</v>
       </c>
       <c r="O87" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P87">
         <v>0</v>
@@ -6562,7 +6562,7 @@
         <v>88</v>
       </c>
       <c r="P89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q89" s="3">
         <v>0</v>
@@ -6689,7 +6689,7 @@
         <v>90</v>
       </c>
       <c r="P91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q91" s="3">
         <v>0</v>
@@ -7079,7 +7079,7 @@
         <v>96</v>
       </c>
       <c r="P97" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q97" s="3">
         <v>0</v>
@@ -7209,7 +7209,7 @@
         <v>98</v>
       </c>
       <c r="P99" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q99" s="3">
         <v>0</v>
@@ -7401,7 +7401,7 @@
         <v>99</v>
       </c>
       <c r="O102" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P102">
         <v>0</v>
@@ -7463,7 +7463,7 @@
         <v>0</v>
       </c>
       <c r="N103" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O103">
         <v>102</v>
@@ -7664,7 +7664,7 @@
         <v>105</v>
       </c>
       <c r="P106" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q106" s="3">
         <v>0</v>
@@ -7794,7 +7794,7 @@
         <v>107</v>
       </c>
       <c r="P108" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q108" s="3">
         <v>0</v>
@@ -8249,7 +8249,7 @@
         <v>114</v>
       </c>
       <c r="P115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q115" s="3">
         <v>0</v>
@@ -8380,7 +8380,7 @@
         <v>116</v>
       </c>
       <c r="P117" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q117" s="3">
         <v>0</v>
@@ -8835,7 +8835,7 @@
         <v>123</v>
       </c>
       <c r="P124" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q124" s="3">
         <v>0</v>
@@ -8965,7 +8965,7 @@
         <v>125</v>
       </c>
       <c r="P126" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q126" s="3">
         <v>0</v>
@@ -9420,7 +9420,7 @@
         <v>132</v>
       </c>
       <c r="P133" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q133" s="3">
         <v>0</v>
@@ -9550,7 +9550,7 @@
         <v>134</v>
       </c>
       <c r="P135" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q135" s="3">
         <v>0</v>
@@ -10005,7 +10005,7 @@
         <v>141</v>
       </c>
       <c r="P142" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q142" s="3">
         <v>0</v>
@@ -10135,7 +10135,7 @@
         <v>143</v>
       </c>
       <c r="P144" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q144" s="3">
         <v>0</v>
@@ -10200,7 +10200,7 @@
         <v>144</v>
       </c>
       <c r="P145" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q145" s="3">
         <v>0</v>
@@ -10653,7 +10653,7 @@
         <v>149</v>
       </c>
       <c r="O152" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P152">
         <v>0</v>

</xml_diff>

<commit_message>
not stopping in correct spot
</commit_message>
<xml_diff>
--- a/TrackModel/trackData/GreenLine.xlsx
+++ b/TrackModel/trackData/GreenLine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/njm130_pitt_edu/Documents/Documents/1140 Trains/trains/TrackModel/trackData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\TrackModel\trackData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{247374CB-8036-4A5A-8CE7-7EEC22481196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692D30C0-0827-4056-AD70-9981F6B87FD4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647A6665-FA60-4BD7-807B-67FD5BA895AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="107">
   <si>
     <t>Line</t>
   </si>
@@ -357,9 +357,6 @@
   </si>
   <si>
     <t>12, 1</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
 </sst>
 </file>
@@ -788,7 +785,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,10 +902,10 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="O2" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -972,10 +969,10 @@
         <v>2</v>
       </c>
       <c r="O3" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q3" s="3">
         <v>0</v>
@@ -1105,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q5" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
goes to pioneer and back to yard at 10x speed
</commit_message>
<xml_diff>
--- a/TrackModel/trackData/GreenLine.xlsx
+++ b/TrackModel/trackData/GreenLine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\TrackModel\trackData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b71eb1e12f3a2cab/Documents/2024-2025/ECE 1140/Git Hub/trains/TrackModel/trackData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647A6665-FA60-4BD7-807B-67FD5BA895AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{647A6665-FA60-4BD7-807B-67FD5BA895AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF29C25-8C94-4DB8-8B27-76EE3E56769E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="107">
   <si>
     <t>Line</t>
   </si>
@@ -784,22 +784,22 @@
   <dimension ref="A1:T152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="102" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P103" sqref="P103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.88671875" style="7"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="7"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="8" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="8" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,7 +861,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>A3</f>
         <v>Green</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ref="A5:A68" si="1">A4</f>
         <v>Green</v>
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1247,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1767,7 +1767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -1962,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2222,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2287,7 +2287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2352,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2677,7 +2677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2742,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2807,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2872,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3067,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3132,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3197,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3262,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f>A35</f>
         <v>Green</v>
@@ -3327,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3522,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3587,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3652,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3717,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3847,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3912,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3977,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4042,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4107,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4172,7 +4172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4237,7 +4237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4302,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4367,7 +4367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4432,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4497,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4562,7 +4562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4627,7 +4627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4692,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4757,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4822,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4887,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4952,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5017,7 +5017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5082,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5147,7 +5147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5212,7 +5212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="str">
         <f t="shared" ref="A69:A132" si="5">A68</f>
         <v>Green</v>
@@ -5277,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5342,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5407,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5472,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5537,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5602,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5667,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5732,7 +5732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5797,7 +5797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5862,7 +5862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5927,7 +5927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5992,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6057,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6122,7 +6122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6187,7 +6187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6252,7 +6252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6317,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6382,7 +6382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6447,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6512,7 +6512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6577,7 +6577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6639,7 +6639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6704,7 +6704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6769,7 +6769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6834,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6899,7 +6899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6964,7 +6964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7029,7 +7029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7094,7 +7094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7159,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7224,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7289,7 +7289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7354,7 +7354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7419,7 +7419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7468,8 +7468,8 @@
       <c r="O103">
         <v>102</v>
       </c>
-      <c r="P103">
-        <v>0</v>
+      <c r="P103" t="s">
+        <v>87</v>
       </c>
       <c r="Q103" s="3">
         <v>0</v>
@@ -7484,7 +7484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7549,7 +7549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7614,7 +7614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7679,7 +7679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7744,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7809,7 +7809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7874,7 +7874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7939,7 +7939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8004,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8069,7 +8069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8134,7 +8134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8199,7 +8199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8264,7 +8264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8330,7 +8330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8395,7 +8395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8460,7 +8460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8525,7 +8525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8590,7 +8590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8655,7 +8655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8720,7 +8720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8785,7 +8785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8850,7 +8850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8915,7 +8915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -8980,7 +8980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -9045,7 +9045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -9110,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -9175,7 +9175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -9240,7 +9240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -9305,7 +9305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -9370,7 +9370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="str">
         <f t="shared" ref="A133:A152" si="9">A132</f>
         <v>Green</v>
@@ -9435,7 +9435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9500,7 +9500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9565,7 +9565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9630,7 +9630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9695,7 +9695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9760,7 +9760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9825,7 +9825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9890,7 +9890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -9955,7 +9955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10020,7 +10020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10085,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10150,7 +10150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10215,7 +10215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10280,7 +10280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10345,7 +10345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10410,7 +10410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10475,7 +10475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10541,7 +10541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>
@@ -10606,7 +10606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Green</v>

</xml_diff>

<commit_message>
25x speed working for stations
</commit_message>
<xml_diff>
--- a/TrackModel/trackData/GreenLine.xlsx
+++ b/TrackModel/trackData/GreenLine.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/njm130_pitt_edu/Documents/Documents/1140 Trains/trains/TrackModel/trackData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b71eb1e12f3a2cab/Documents/2024-2025/ECE 1140/Git Hub/trains/TrackModel/trackData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{647A6665-FA60-4BD7-807B-67FD5BA895AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83140386-D68A-4825-AF35-22424B921FBD}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{647A6665-FA60-4BD7-807B-67FD5BA895AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{281E65B0-EEC2-40F9-92FB-AB218D3E7E10}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9B511C03-6C71-48AB-BE22-1C54007507AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="107">
   <si>
     <t>Line</t>
   </si>
@@ -363,7 +363,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +385,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -413,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -441,6 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,8 +791,8 @@
   <dimension ref="A1:T153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="102" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M153" sqref="M153"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S101" sqref="S101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7468,8 +7475,8 @@
       <c r="O103">
         <v>102</v>
       </c>
-      <c r="P103">
-        <v>0</v>
+      <c r="P103" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="Q103" s="3">
         <v>0</v>
@@ -10735,7 +10742,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:T153">
+  <conditionalFormatting sqref="I2:T102 I104:T153 I103:O103 Q103:T103">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>